<commit_message>
update countries for mental health
</commit_message>
<xml_diff>
--- a/poverty.xlsx
+++ b/poverty.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anamakarevich/UdacityProjects/suicide_rates_factors/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFAE9D77-C08B-824A-AFAC-53D541D08950}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DD526A6-172D-B041-B518-FAFF68B110F3}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -298,9 +298,6 @@
     <t xml:space="preserve"> Vanuatu</t>
   </si>
   <si>
-    <t xml:space="preserve"> Viet Nam</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Yemen</t>
   </si>
   <si>
@@ -332,6 +329,9 @@
   </si>
   <si>
     <t xml:space="preserve"> Cote d'Ivoire</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Vietnam</t>
   </si>
 </sst>
 </file>
@@ -692,8 +692,8 @@
   </sheetPr>
   <dimension ref="A1:C103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
+      <selection activeCell="B101" sqref="B101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -817,7 +817,7 @@
         <v>118</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -942,7 +942,7 @@
         <v>176</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C26" s="1">
         <v>0.36899999999999999</v>
@@ -953,7 +953,7 @@
         <v>171</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1188,7 +1188,7 @@
         <v>138</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C50" s="1">
         <v>0.186</v>
@@ -1286,7 +1286,7 @@
         <v>107</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C60" s="1">
         <v>4.0000000000000001E-3</v>
@@ -1404,7 +1404,7 @@
         <v>114</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C71" s="1">
         <v>5.0000000000000001E-3</v>
@@ -1570,7 +1570,7 @@
         <v>151</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="13" x14ac:dyDescent="0.15">
@@ -1586,7 +1586,7 @@
         <v>82</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C90" s="1">
         <v>7.0000000000000001E-3</v>
@@ -1681,7 +1681,7 @@
         <v>115</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="C100" s="1">
         <v>1.6E-2</v>
@@ -1692,7 +1692,7 @@
         <v>168</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C101" s="1">
         <v>0.2</v>
@@ -1703,7 +1703,7 @@
         <v>139</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C102" s="1">
         <v>0.26400000000000001</v>
@@ -1714,7 +1714,7 @@
         <v>154</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C103" s="1">
         <v>0.128</v>

</xml_diff>